<commit_message>
files: constants from initial values
</commit_message>
<xml_diff>
--- a/output/new_york_times_scraper.xlsx
+++ b/output/new_york_times_scraper.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>title</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Is Tucker Carlson Too Hot for Twitter to Handle?</t>
-  </si>
-  <si>
-    <t>11h ago</t>
   </si>
   <si>
     <t>Elon Musk didn't exactly give the conservative media star a warm embrace, suggesting the outspoken owner has reservations.</t>
@@ -652,16 +649,16 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
       </c>
       <c r="F6">
         <v>27</v>
@@ -672,19 +669,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
       <c r="F7">
         <v>30</v>
@@ -695,19 +692,19 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
       </c>
       <c r="F8">
         <v>33</v>
@@ -718,19 +715,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" t="s">
         <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>46</v>
       </c>
       <c r="F9">
         <v>30</v>
@@ -741,19 +738,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" t="s">
         <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
       </c>
       <c r="F10">
         <v>31</v>
@@ -764,19 +761,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
       </c>
       <c r="F11">
         <v>30</v>

</xml_diff>